<commit_message>
added led logic, full uart logic, added calibration for temp and humidity sensor but that's still finicky
</commit_message>
<xml_diff>
--- a/l475_disco_pins.xlsx
+++ b/l475_disco_pins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\EE2028_stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwx\Documents\Github\EE2028_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61283A8E-C959-431E-A409-39F29E681B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E71C94-6790-4326-8B75-FEFBF46F268E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4ED1FEC-F547-459C-82B1-90387225173E}"/>
+    <workbookView xWindow="38850" yWindow="5355" windowWidth="16350" windowHeight="15345" xr2:uid="{B4ED1FEC-F547-459C-82B1-90387225173E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>PIN ASSIGNMENTS</t>
   </si>
@@ -461,9 +461,6 @@
     <t>PA2</t>
   </si>
   <si>
-    <t>SPI_SSN</t>
-  </si>
-  <si>
     <t>GPIO-PA3</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
     <t>SPI1_MOSI</t>
   </si>
   <si>
-    <t>PWM</t>
-  </si>
-  <si>
     <t>PA7</t>
   </si>
   <si>
@@ -560,9 +554,6 @@
     <t>PB8</t>
   </si>
   <si>
-    <t>LED1</t>
-  </si>
-  <si>
     <t>A5</t>
   </si>
   <si>
@@ -584,7 +575,64 @@
     <t>LPTIM1_IN1/LPTIM2_IN2/I2C3_SCL/LPUART1_RX</t>
   </si>
   <si>
-    <t>PUSHBUTTON</t>
+    <t>TIM1C2,TIM3C3,TIM8C2N</t>
+  </si>
+  <si>
+    <t>TIM2C2,TIM5C2,TIM15C1N,UART4RX</t>
+  </si>
+  <si>
+    <t>TIM2C4,TIM5C4,TIM15C2,UART2RX</t>
+  </si>
+  <si>
+    <t>TIM2C1,TIM5C1,UART4TX</t>
+  </si>
+  <si>
+    <t>T2C3,T5C3,T15C1,UART2TX</t>
+  </si>
+  <si>
+    <t>USART2CK,SPI1NSS,SPI3NSS</t>
+  </si>
+  <si>
+    <t>T1C3N,T3C4,T8C3N</t>
+  </si>
+  <si>
+    <t>T3C1,SPI1MISO,SPI3MISO</t>
+  </si>
+  <si>
+    <t>I2C3_SMBA</t>
+  </si>
+  <si>
+    <t>T2C1,SPI1NSS,SPI3NSS</t>
+  </si>
+  <si>
+    <t>T3C1,T16C1,SPI1MISO</t>
+  </si>
+  <si>
+    <t>T1C1N,T3C2,T8C1N,T17C1,SPI1MOSI</t>
+  </si>
+  <si>
+    <t>T2C1,T8C1,SPI1SCK</t>
+  </si>
+  <si>
+    <t>T4C3,T16C1,I2C1SCL</t>
+  </si>
+  <si>
+    <t>T4C4,T17C1,CAN1TX,I2C1SDA,SPI2NSS</t>
+  </si>
+  <si>
+    <t>T4C3</t>
+  </si>
+  <si>
+    <t>USART3TX</t>
+  </si>
+  <si>
+    <t>USART3RX</t>
+  </si>
+  <si>
+    <t>T3C4,T8C4</t>
+  </si>
+  <si>
+    <t>T1C2N,T8C2N,T15C1,I2C2SDA,SPI2MISO</t>
   </si>
 </sst>
 </file>
@@ -975,19 +1023,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17600CA4-236E-49FA-8FEC-56C9C2DEC62E}">
   <dimension ref="A3:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -997,7 +1045,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
@@ -1009,7 +1057,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>68</v>
@@ -1019,7 +1067,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
@@ -1031,7 +1079,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1041,7 +1089,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1053,7 +1101,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -1063,7 +1111,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
@@ -1073,7 +1121,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -1083,7 +1131,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
@@ -1093,7 +1141,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
@@ -1103,7 +1151,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1115,7 +1163,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>44</v>
@@ -1125,7 +1173,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>45</v>
@@ -1135,7 +1183,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
@@ -1147,7 +1195,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
         <v>31</v>
@@ -1157,7 +1205,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="2" t="s">
         <v>34</v>
@@ -1167,7 +1215,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
         <v>36</v>
@@ -1177,7 +1225,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>37</v>
@@ -1187,7 +1235,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1199,7 +1247,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>51</v>
@@ -1209,7 +1257,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
         <v>53</v>
@@ -1219,7 +1267,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>55</v>
       </c>
@@ -1231,7 +1279,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
         <v>58</v>
@@ -1241,7 +1289,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="2" t="s">
         <v>59</v>
@@ -1251,7 +1299,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>62</v>
       </c>
@@ -1263,7 +1311,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
         <v>65</v>
@@ -1273,7 +1321,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1285,7 +1333,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>76</v>
       </c>
@@ -1297,7 +1345,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>78</v>
       </c>
@@ -1309,7 +1357,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>82</v>
       </c>
@@ -1321,7 +1369,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>85</v>
       </c>
@@ -1333,7 +1381,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="2" t="s">
         <v>88</v>
@@ -1343,7 +1391,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>93</v>
       </c>
@@ -1355,7 +1403,7 @@
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="2" t="s">
         <v>97</v>
@@ -1365,7 +1413,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="2" t="s">
         <v>99</v>
@@ -1375,7 +1423,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="2" t="s">
         <v>101</v>
@@ -1387,7 +1435,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="2" t="s">
         <v>105</v>
@@ -1399,7 +1447,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="2" t="s">
         <v>107</v>
@@ -1411,7 +1459,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="2" t="s">
         <v>111</v>
@@ -1421,7 +1469,7 @@
       </c>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>90</v>
       </c>
@@ -1433,7 +1481,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="2" t="s">
         <v>91</v>
@@ -1441,9 +1489,11 @@
       <c r="C44" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="2" t="s">
         <v>33</v>
@@ -1451,43 +1501,47 @@
       <c r="C45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>113</v>
       </c>
@@ -1495,11 +1549,13 @@
         <v>118</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>114</v>
       </c>
@@ -1510,10 +1566,10 @@
         <v>14</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>115</v>
       </c>
@@ -1524,10 +1580,10 @@
         <v>13</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>116</v>
       </c>
@@ -1538,12 +1594,12 @@
         <v>12</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>7</v>
@@ -1552,10 +1608,10 @@
         <v>8</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>119</v>
       </c>
@@ -1565,9 +1621,11 @@
       <c r="C54" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>120</v>
       </c>
@@ -1577,105 +1635,123 @@
       <c r="C55" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>129</v>
       </c>
@@ -1686,88 +1762,84 @@
         <v>140</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="D69" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A24"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A8:A13"/>
@@ -1775,6 +1847,11 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>